<commit_message>
Documentation and bug fixing
</commit_message>
<xml_diff>
--- a/tests/data/sensitivities/config/design_input_onebyone.xlsx
+++ b/tests/data/sensitivities/config/design_input_onebyone.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" state="visible" r:id="rId2"/>
@@ -259,28 +259,16 @@
       <text>
         <r>
           <rPr>
-            <b val="true"/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Trine Alsos:
-If background spreadsheet exists a set of background parameters is sampled from these distributions. 
-The number of samples = max(generalinput. repeats , designinput.numreals)
+          <t>The set of background parameters is sampled from these distributions. 
+The number of samples = max(general_input. repeats , designinput.numreals)
 The table of sampled values are kept the same for all single sensitivities.
-This means that for the sensitivities where a parameter is not “in focus”  the parameter values will be taken from the background table if it exists there.  If parameter does not exist in background table , parameter defaultvalues are used instead.</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Distributions and order og distribution parameters are the same as in design input spreadsheet.</t>
+This means that for the sensitivities where a parameter is not “in focus”  the parameter values will be taken from the background table if it exists there.  If parameter does not exist in background table , parameter defaultvalues are used instead.Distributions and order of distribution parameters are the same as in design input spreadsheet.</t>
         </r>
       </text>
     </comment>
@@ -289,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
   <si>
     <t>designtype</t>
   </si>
@@ -1960,7 +1948,7 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2969,20 +2957,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O16" activeCellId="0" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.1173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5816326530612"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.83673469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.219387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.83673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.219387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3002,9 +2991,12 @@
         <v>18</v>
       </c>
       <c r="F1" s="185" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="185" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="186" t="s">
+      <c r="H1" s="186" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3022,10 +3014,11 @@
         <v>1</v>
       </c>
       <c r="E2" s="189"/>
-      <c r="F2" s="189" t="n">
+      <c r="F2" s="189"/>
+      <c r="G2" s="189" t="n">
         <v>2</v>
       </c>
-      <c r="G2" s="155" t="s">
+      <c r="H2" s="155" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3043,10 +3036,11 @@
         <v>1</v>
       </c>
       <c r="E3" s="192"/>
-      <c r="F3" s="192" t="n">
+      <c r="F3" s="192"/>
+      <c r="G3" s="192" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="193"/>
+      <c r="H3" s="193"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="190" t="s">
@@ -3064,10 +3058,11 @@
       <c r="E4" s="192" t="n">
         <v>5</v>
       </c>
-      <c r="F4" s="192" t="n">
+      <c r="F4" s="192"/>
+      <c r="G4" s="192" t="n">
         <v>2</v>
       </c>
-      <c r="G4" s="193"/>
+      <c r="H4" s="193"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Use pytest tmpdir for fmudesign endpoint testing (#18)
Include blackening the file.

Using pytest avoids repo-clutter.

Reorganize slightly files vs test-functions
</commit_message>
<xml_diff>
--- a/tests/data/sensitivities/config/design_input_onebyone.xlsx
+++ b/tests/data/sensitivities/config/design_input_onebyone.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,13 +16,18 @@
     <sheet name="background_corr" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -35,7 +40,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Specifies that this is a setup for a onebyone design and not a design of morris type</t>
+          <t xml:space="preserve">Specifies that this is a setup for a onebyone design and not a design of morris type</t>
         </r>
       </text>
     </comment>
@@ -49,7 +54,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Number of repeated seeds per sensitivity/sensitivity case. 
+          <t xml:space="preserve">Number of repeated seeds per sensitivity/sensitivity case. 
 This is overrided if number of realisations is specified in the numreal column in designinput.</t>
         </r>
       </text>
@@ -64,7 +69,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Alternatives:
+          <t xml:space="preserve">Alternatives:
 - default gives seed numbers 1000, 1001, 1002, 1003,---
 - None (seed number is not added as parameter in spreadsheet) 
 - filename for file with list of seeds in ert/input/distributions/If only one seed is given in the external seed file, this is used for all realisations – NOT IMPLEMENTED YET</t>
@@ -81,7 +86,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Alternatives:
+          <t xml:space="preserve">Alternatives:
 - None
 - name of sheet in this workbook with background parameters
 - Name of external file with background parameters. Must end with .xlsx or .csv and be readable as pandas dataframe with parameter names as column headers.
@@ -96,7 +101,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -110,7 +115,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Trine Alsos:</t>
+          <t xml:space="preserve">Trine Alsos:</t>
         </r>
         <r>
           <rPr>
@@ -120,7 +125,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>numreal = repeats if not specified in table</t>
+          <t xml:space="preserve">numreal = repeats if not specified in table</t>
         </r>
       </text>
     </comment>
@@ -135,7 +140,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Trine Alsos:
+          <t xml:space="preserve">Trine Alsos:
 For case sensitivities</t>
         </r>
         <r>
@@ -146,7 +151,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>provide names for case1 and case2 and values. Values can be string</t>
+          <t xml:space="preserve">provide names for case1 and case2 and values. Values can be string</t>
         </r>
       </text>
     </comment>
@@ -161,7 +166,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Trine Alsos:
+          <t xml:space="preserve">Trine Alsos:
 Distname and dist_param1, .. only for p10_p90 sensitivities or background parameters</t>
         </r>
         <r>
@@ -172,7 +177,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Order of distribution parameters must be predefines (and where applicable, same as used for ert in GEN_KW)
+          <t xml:space="preserve">Order of distribution parameters must be predefines (and where applicable, same as used for ert in GEN_KW)
 e.g. 
 normal(mean, std dev,min, max) – where min/max is optional and will give truncated gaussian
 lognormal(mean, stddev, min, max) – where min/max is optional and will give truncated lognormal
@@ -191,7 +196,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Outcomes, split with comma</t>
+          <t xml:space="preserve">Outcomes, split with comma</t>
         </r>
       </text>
     </comment>
@@ -205,7 +210,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>fractions</t>
+          <t xml:space="preserve">fractions</t>
         </r>
       </text>
     </comment>
@@ -216,7 +221,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -230,7 +235,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Trine Alsos:</t>
+          <t xml:space="preserve">Trine Alsos:</t>
         </r>
         <r>
           <rPr>
@@ -240,7 +245,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Used both as default and as base case value for single sensitivities.
+          <t xml:space="preserve">Used both as default and as base case value for single sensitivities.
 Values can be strings or numbers</t>
         </r>
       </text>
@@ -252,7 +257,7 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -265,7 +270,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>The set of background parameters is sampled from these distributions. 
+          <t xml:space="preserve">The set of background parameters is sampled from these distributions. 
 The number of samples = max(general_input. repeats , designinput.numreals)
 The table of sampled values are kept the same for all single sensitivities.
 This means that for the sensitivities where a parameter is not “in focus”  the parameter values will be taken from the background table if it exists there.  If parameter does not exist in background table , parameter defaultvalues are used instead.Distributions and order of distribution parameters are the same as in design input spreadsheet.</t>
@@ -277,258 +282,255 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="84">
-  <si>
-    <t>designtype</t>
-  </si>
-  <si>
-    <t>onebyone</t>
-  </si>
-  <si>
-    <t>repeats</t>
-  </si>
-  <si>
-    <t>rms_seeds</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>background</t>
-  </si>
-  <si>
-    <t>./tests/data/sensitivities/config/doe1.xlsx</t>
-  </si>
-  <si>
-    <t>sensname</t>
-  </si>
-  <si>
-    <t>numreal</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>param_name</t>
-  </si>
-  <si>
-    <t>senscase1</t>
-  </si>
-  <si>
-    <t>value1</t>
-  </si>
-  <si>
-    <t>senscase2</t>
-  </si>
-  <si>
-    <t>value2</t>
-  </si>
-  <si>
-    <t>dist_name</t>
-  </si>
-  <si>
-    <t>dist_param1</t>
-  </si>
-  <si>
-    <t>dist_param2</t>
-  </si>
-  <si>
-    <t>dist_param3</t>
-  </si>
-  <si>
-    <t>dist_param4</t>
-  </si>
-  <si>
-    <t>decimals</t>
-  </si>
-  <si>
-    <t>corr_sheet</t>
-  </si>
-  <si>
-    <t>extern_file</t>
-  </si>
-  <si>
-    <t>seed</t>
-  </si>
-  <si>
-    <t>faults</t>
-  </si>
-  <si>
-    <t>scenario</t>
-  </si>
-  <si>
-    <t>PARAM1</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
-    <t>velmodel</t>
-  </si>
-  <si>
-    <t>DC_MODEL</t>
-  </si>
-  <si>
-    <t>alternative</t>
-  </si>
-  <si>
-    <t>contacts</t>
-  </si>
-  <si>
-    <t>PARAM2</t>
-  </si>
-  <si>
-    <t>shallow</t>
-  </si>
-  <si>
-    <t>deep</t>
-  </si>
-  <si>
-    <t>PARAM3</t>
-  </si>
-  <si>
-    <t>PARAM4</t>
-  </si>
-  <si>
-    <t>multz</t>
-  </si>
-  <si>
-    <t>dist</t>
-  </si>
-  <si>
-    <t>MULTZ_ILE</t>
-  </si>
-  <si>
-    <t>logunif</t>
-  </si>
-  <si>
-    <t>0.0001</t>
-  </si>
-  <si>
-    <t>sens6</t>
-  </si>
-  <si>
-    <t>PARAM5</t>
-  </si>
-  <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>PARAM6</t>
-  </si>
-  <si>
-    <t>uniform</t>
-  </si>
-  <si>
-    <t>PARAM7</t>
-  </si>
-  <si>
-    <t>triang</t>
-  </si>
-  <si>
-    <t>FAULT_SEAL</t>
-  </si>
-  <si>
-    <t>discrete</t>
-  </si>
-  <si>
-    <t>2018-11-02, 2018-11-03, 2018-11-04</t>
-  </si>
-  <si>
-    <t>0.3, 0.4, 0.3</t>
-  </si>
-  <si>
-    <t>sens7</t>
-  </si>
-  <si>
-    <t>PARAM9</t>
-  </si>
-  <si>
-    <t>lognormal</t>
-  </si>
-  <si>
-    <t>corr1</t>
-  </si>
-  <si>
-    <t>PARAM10</t>
-  </si>
-  <si>
-    <t>PARAM11</t>
-  </si>
-  <si>
-    <t>PARAM12</t>
-  </si>
-  <si>
-    <t>sens8</t>
-  </si>
-  <si>
-    <t>extern</t>
-  </si>
-  <si>
-    <t>PARAM13</t>
-  </si>
-  <si>
-    <t>tests/data/sensitivities/config/doe1.xlsx</t>
-  </si>
-  <si>
-    <t>PARAM14</t>
-  </si>
-  <si>
-    <t>PARAM15</t>
-  </si>
-  <si>
-    <t>PARAM16</t>
-  </si>
-  <si>
-    <t>default_value</t>
-  </si>
-  <si>
-    <t>DEFAULT1</t>
-  </si>
-  <si>
-    <t>DEFAULT2</t>
-  </si>
-  <si>
-    <t>prediction</t>
-  </si>
-  <si>
-    <t>DEFAULT3</t>
-  </si>
-  <si>
-    <t>base</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>PARAM8</t>
-  </si>
-  <si>
-    <t>PARAM17</t>
-  </si>
-  <si>
-    <t>PARAM18</t>
-  </si>
-  <si>
-    <t>PARAM19</t>
-  </si>
-  <si>
-    <t>0.9</t>
-  </si>
-  <si>
-    <t>PARAM20</t>
-  </si>
-  <si>
-    <t>background_corr</t>
-  </si>
-  <si>
-    <t>PARAM21</t>
-  </si>
-  <si>
-    <t>PARAM22</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
+  <si>
+    <t xml:space="preserve">designtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">onebyone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">repeats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rms_seeds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">background</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doe1.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numreal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">param_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">senscase1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">senscase2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dist_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dist_param1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dist_param2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dist_param3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dist_param4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corr_sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extern_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">faults</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">velmodel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC_MODEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alternative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contacts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shallow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MULTZ_ILE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logunif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sens6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uniform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAULT_SEAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">discrete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-11-02, 2018-11-03, 2018-11-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3, 0.4, 0.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sens7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lognormal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corr1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sens8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFAULT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFAULT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prediction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFAULT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">background_corr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAM22</t>
   </si>
 </sst>
 </file>
@@ -536,7 +538,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -1873,12 +1875,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1950,16 +1952,15 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.8622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="77.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1998,7 +1999,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2014,27 +2015,24 @@
   </sheetPr>
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K15" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P17" activeCellId="0" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8622448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="10"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="2" width="11.8622448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8622448979592"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="33.1173469387755"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="2" width="11.8622448979592"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="11.8622448979592"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.72959183673469"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="2" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="33.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="2" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="9.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2547,7 +2545,7 @@
       <c r="N17" s="118"/>
       <c r="O17" s="172"/>
       <c r="P17" s="119" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2555,7 +2553,7 @@
       <c r="B18" s="121"/>
       <c r="C18" s="122"/>
       <c r="D18" s="123" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E18" s="173"/>
       <c r="F18" s="174"/>
@@ -2575,7 +2573,7 @@
       <c r="B19" s="121"/>
       <c r="C19" s="122"/>
       <c r="D19" s="123" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E19" s="173"/>
       <c r="F19" s="174"/>
@@ -2595,7 +2593,7 @@
       <c r="B20" s="133"/>
       <c r="C20" s="134"/>
       <c r="D20" s="135" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" s="177"/>
       <c r="F20" s="178"/>
@@ -2613,7 +2611,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2629,15 +2627,14 @@
   </sheetPr>
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="13.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.72959183673469"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="13.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2645,12 +2642,12 @@
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>0</v>
@@ -2658,15 +2655,15 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>0</v>
@@ -2685,7 +2682,7 @@
         <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2717,7 +2714,7 @@
         <v>40</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2746,7 +2743,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>0</v>
@@ -2794,7 +2791,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>0</v>
@@ -2802,7 +2799,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>0</v>
@@ -2810,7 +2807,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="2" t="n">
         <v>0</v>
@@ -2818,7 +2815,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>0</v>
@@ -2826,7 +2823,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>0</v>
@@ -2834,7 +2831,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>0</v>
@@ -2845,14 +2842,14 @@
         <v>50</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2868,14 +2865,11 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
@@ -2907,7 +2901,7 @@
         <v>58</v>
       </c>
       <c r="B3" s="181" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="181" t="n">
         <v>1</v>
@@ -2923,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="181" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D4" s="181" t="n">
         <v>1</v>
@@ -2950,7 +2944,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2965,19 +2959,16 @@
   </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.83673469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.219387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3008,7 +2999,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="187" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="188" t="s">
         <v>45</v>
@@ -3025,12 +3016,12 @@
         <v>2</v>
       </c>
       <c r="H2" s="155" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="190" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="191" t="s">
         <v>47</v>
@@ -3050,7 +3041,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="190" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="191" t="s">
         <v>49</v>
@@ -3073,7 +3064,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3089,29 +3080,26 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="181" t="n">
         <v>1</v>
@@ -3121,10 +3109,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="181" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="181" t="n">
         <v>1</v>
@@ -3133,13 +3121,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="181" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="181" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D4" s="181" t="n">
         <v>1</v>
@@ -3148,7 +3136,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>